<commit_message>
removed some channel maps for better coverage
want some channels to not be in the channel map
</commit_message>
<xml_diff>
--- a/test/inputs/biotek.xlsx
+++ b/test/inputs/biotek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{2B5EB8AA-8848-0143-B17F-D0507D34053E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AE93200-9096-864A-B1F1-525AC8DADF25}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{2B5EB8AA-8848-0143-B17F-D0507D34053E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B4F0F16-2D60-F04D-AD98-689443334844}"/>
   <bookViews>
-    <workbookView xWindow="11180" yWindow="880" windowWidth="18980" windowHeight="9440" activeTab="1" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="20580" yWindow="7480" windowWidth="18980" windowHeight="9440" activeTab="1" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Plate</t>
   </si>
@@ -100,15 +100,6 @@
   </si>
   <si>
     <t>od2</t>
-  </si>
-  <si>
-    <t>flu1</t>
-  </si>
-  <si>
-    <t>485,530[2]</t>
-  </si>
-  <si>
-    <t>flu2</t>
   </si>
 </sst>
 </file>
@@ -549,10 +540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA707B9-0BE9-45E5-A5EE-A3873F0594F1}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -585,20 +576,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>485530</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix channel map (#27)
* fix channel map for biotek and spectramax

* update tests

* add error tests for coverage

* removed some channel maps for better coverage

want some channels to not be in the channel map

* i am stupid

channel map includes all channels, even the option for them staying the same
removing error catching that isn't needed
</commit_message>
<xml_diff>
--- a/test/inputs/biotek.xlsx
+++ b/test/inputs/biotek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{2B5EB8AA-8848-0143-B17F-D0507D34053E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AE93200-9096-864A-B1F1-525AC8DADF25}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{2B5EB8AA-8848-0143-B17F-D0507D34053E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B4F0F16-2D60-F04D-AD98-689443334844}"/>
   <bookViews>
-    <workbookView xWindow="11180" yWindow="880" windowWidth="18980" windowHeight="9440" activeTab="1" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="20580" yWindow="7480" windowWidth="18980" windowHeight="9440" activeTab="1" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Plate</t>
   </si>
@@ -100,15 +100,6 @@
   </si>
   <si>
     <t>od2</t>
-  </si>
-  <si>
-    <t>flu1</t>
-  </si>
-  <si>
-    <t>485,530[2]</t>
-  </si>
-  <si>
-    <t>flu2</t>
   </si>
 </sst>
 </file>
@@ -549,10 +540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA707B9-0BE9-45E5-A5EE-A3873F0594F1}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -585,20 +576,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>485530</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed spec and biotek.xlsx to match
</commit_message>
<xml_diff>
--- a/test/inputs/biotek.xlsx
+++ b/test/inputs/biotek.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{2B5EB8AA-8848-0143-B17F-D0507D34053E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B4F0F16-2D60-F04D-AD98-689443334844}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4042B1F-748B-B646-9293-122223345008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20580" yWindow="7480" windowWidth="18980" windowHeight="9440" activeTab="1" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="19420" yWindow="7480" windowWidth="18980" windowHeight="9440" activeTab="4" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
-    <sheet name="ID" sheetId="5" r:id="rId2"/>
+    <sheet name="Channel Map" sheetId="5" r:id="rId2"/>
     <sheet name="Groups" sheetId="2" r:id="rId3"/>
     <sheet name="Transformations" sheetId="3" r:id="rId4"/>
     <sheet name="Views" sheetId="4" r:id="rId5"/>
@@ -51,9 +51,6 @@
     <t>Well</t>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -66,15 +63,6 @@
     <t>Equation</t>
   </si>
   <si>
-    <t>Groups</t>
-  </si>
-  <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
     <t>Plate brand</t>
   </si>
   <si>
@@ -100,6 +88,18 @@
   </si>
   <si>
     <t>od2</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>New name</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>View</t>
   </si>
 </sst>
 </file>
@@ -482,54 +482,54 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
         <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA707B9-0BE9-45E5-A5EE-A3873F0594F1}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -553,26 +553,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -588,7 +588,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B29"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -601,7 +601,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -625,10 +625,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -640,18 +640,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>